<commit_message>
AB Bug Fixes - NL Data Updates
</commit_message>
<xml_diff>
--- a/docs/NL-Datasets-Attributes.xlsx
+++ b/docs/NL-Datasets-Attributes.xlsx
@@ -3506,10 +3506,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EW108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EL1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="EW109" sqref="EW109:EW111"/>
+      <selection pane="bottomLeft" activeCell="Y78" sqref="Y78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3552,7 +3552,9 @@
     <col min="41" max="41" width="25.5703125" style="1" customWidth="1"/>
     <col min="42" max="42" width="25" customWidth="1"/>
     <col min="43" max="43" width="23.5703125" customWidth="1"/>
-    <col min="44" max="51" width="24.140625" customWidth="1"/>
+    <col min="44" max="44" width="24.140625" customWidth="1"/>
+    <col min="45" max="45" width="91.28515625" customWidth="1"/>
+    <col min="46" max="51" width="24.140625" customWidth="1"/>
     <col min="52" max="52" width="24.140625" style="1" customWidth="1"/>
     <col min="53" max="64" width="24.140625" customWidth="1"/>
     <col min="65" max="65" width="24.7109375" customWidth="1"/>
@@ -10088,7 +10090,7 @@
       <c r="AR37" t="s">
         <v>159</v>
       </c>
-      <c r="AS37" t="s">
+      <c r="AS37" s="5" t="s">
         <v>350</v>
       </c>
       <c r="EE37" t="s">
@@ -21411,7 +21413,7 @@
       <c r="AR75" t="s">
         <v>159</v>
       </c>
-      <c r="AS75" t="s">
+      <c r="AS75" s="5" t="s">
         <v>774</v>
       </c>
       <c r="AT75" t="s">
@@ -21906,7 +21908,7 @@
       <c r="AR78" t="s">
         <v>159</v>
       </c>
-      <c r="AS78" t="s">
+      <c r="AS78" s="5" t="s">
         <v>809</v>
       </c>
       <c r="AT78" t="s">
@@ -27124,6 +27126,9 @@
     <hyperlink ref="Y78" r:id="rId71"/>
     <hyperlink ref="Y91" r:id="rId72"/>
     <hyperlink ref="Y90" r:id="rId73"/>
+    <hyperlink ref="AS75" r:id="rId74"/>
+    <hyperlink ref="AS78" r:id="rId75"/>
+    <hyperlink ref="AS37" r:id="rId76"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>